<commit_message>
Adding updated utils, tests, and pom
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/excel/signup_acc_info.xlsx
+++ b/src/test/resources/testdata/excel/signup_acc_info.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="174">
   <si>
     <t>title</t>
   </si>
@@ -496,6 +496,45 @@
   </si>
   <si>
     <t>209-655-5393</t>
+  </si>
+  <si>
+    <t>Luke</t>
+  </si>
+  <si>
+    <t>jaclyn.brakus@yahoo.com</t>
+  </si>
+  <si>
+    <t>jvwawaqlmm75td</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>Botsford</t>
+  </si>
+  <si>
+    <t>Carter-Sporer</t>
+  </si>
+  <si>
+    <t>4820 Foster Way</t>
+  </si>
+  <si>
+    <t>Suite 808</t>
+  </si>
+  <si>
+    <t>Israel</t>
+  </si>
+  <si>
+    <t>Nebraska</t>
+  </si>
+  <si>
+    <t>Port Quinn</t>
+  </si>
+  <si>
+    <t>47200</t>
+  </si>
+  <si>
+    <t>807-647-6977</t>
   </si>
 </sst>
 </file>
@@ -748,7 +787,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:S8"/>
+  <dimension ref="A1:S9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1183,6 +1222,65 @@
       <c r="E8" t="s" s="0">
         <v>150</v>
       </c>
+      <c r="F8" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="G8" t="s" s="0">
+        <v>109</v>
+      </c>
+      <c r="H8" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="I8" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="J8" t="s" s="0">
+        <v>161</v>
+      </c>
+      <c r="K8" t="s" s="0">
+        <v>165</v>
+      </c>
+      <c r="L8" t="s" s="0">
+        <v>166</v>
+      </c>
+      <c r="M8" t="s" s="0">
+        <v>167</v>
+      </c>
+      <c r="N8" t="s" s="0">
+        <v>168</v>
+      </c>
+      <c r="O8" t="s" s="0">
+        <v>169</v>
+      </c>
+      <c r="P8" t="s" s="0">
+        <v>170</v>
+      </c>
+      <c r="Q8" t="s" s="0">
+        <v>171</v>
+      </c>
+      <c r="R8" t="s" s="0">
+        <v>172</v>
+      </c>
+      <c r="S8" t="s" s="0">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s" s="0">
+        <v>161</v>
+      </c>
+      <c r="C9" t="s" s="0">
+        <v>162</v>
+      </c>
+      <c r="D9" t="s" s="0">
+        <v>163</v>
+      </c>
+      <c r="E9" t="s" s="0">
+        <v>164</v>
+      </c>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>